<commit_message>
Deleted old and now unused files and folders from Norway folder
</commit_message>
<xml_diff>
--- a/paper3_JacksonBlake_etal/WindowsOfOpportunity_Responses.xlsx
+++ b/paper3_JacksonBlake_etal/WindowsOfOpportunity_Responses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\seasonal_forecasting_watexr\paper3_JacksonBlake_etal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE161BA-F305-4B66-9E5F-874D88A11615}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872B2BAE-D1AC-46C1-A0F1-0ED64B1F49C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{165BE1C7-909E-42BB-BD38-F3EE9C9CA183}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{165BE1C7-909E-42BB-BD38-F3EE9C9CA183}"/>
   </bookViews>
   <sheets>
     <sheet name="Spain" sheetId="1" r:id="rId1"/>
@@ -1149,21 +1149,109 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1173,132 +1261,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1652,7 +1652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6D43E3-980E-4F4E-8547-FE8A35AE7044}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2065,13 +2065,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C981C5-1431-4C78-9739-6374280083DD}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.42578125" customWidth="1"/>
+    <col min="1" max="1" width="155.85546875" customWidth="1"/>
     <col min="2" max="2" width="37.7109375" customWidth="1"/>
     <col min="3" max="3" width="50.85546875" customWidth="1"/>
   </cols>
@@ -2970,22 +2970,22 @@
       <c r="B1" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="59" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="32"/>
+      <c r="F1" s="59"/>
       <c r="G1" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="59" t="s">
         <v>177</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
@@ -3187,26 +3187,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="64" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="62" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="60" t="s">
         <v>205</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
       <c r="D2" s="23" t="s">
         <v>165</v>
       </c>
@@ -3221,10 +3221,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="64" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="62" t="s">
         <v>198</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -3236,8 +3236,8 @@
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="34"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
       <c r="C4" s="10" t="s">
         <v>171</v>
       </c>
@@ -3249,8 +3249,8 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
-      <c r="B5" s="38"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="13" t="s">
         <v>172</v>
       </c>
@@ -3260,8 +3260,8 @@
       <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
-      <c r="B6" s="39" t="s">
+      <c r="A6" s="66"/>
+      <c r="B6" s="69" t="s">
         <v>199</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -3275,8 +3275,8 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="10" t="s">
         <v>171</v>
       </c>
@@ -3286,8 +3286,8 @@
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
-      <c r="B8" s="38"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="13" t="s">
         <v>172</v>
       </c>
@@ -3301,8 +3301,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
-      <c r="B9" s="39" t="s">
+      <c r="A9" s="66"/>
+      <c r="B9" s="69" t="s">
         <v>200</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -3314,8 +3314,8 @@
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
-      <c r="B10" s="37"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="10" t="s">
         <v>171</v>
       </c>
@@ -3325,8 +3325,8 @@
       <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
-      <c r="B11" s="38"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="68"/>
       <c r="C11" s="13" t="s">
         <v>172</v>
       </c>
@@ -3338,8 +3338,8 @@
       <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
-      <c r="B12" s="37" t="s">
+      <c r="A12" s="66"/>
+      <c r="B12" s="67" t="s">
         <v>201</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -3353,8 +3353,8 @@
       <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
-      <c r="B13" s="37"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="10" t="s">
         <v>171</v>
       </c>
@@ -3364,8 +3364,8 @@
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="40"/>
+      <c r="A14" s="65"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="19" t="s">
         <v>172</v>
       </c>
@@ -3375,10 +3375,10 @@
       <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="64" t="s">
         <v>169</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="62" t="s">
         <v>198</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -3390,8 +3390,8 @@
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
-      <c r="B16" s="37"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="10" t="s">
         <v>171</v>
       </c>
@@ -3401,8 +3401,8 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
-      <c r="B17" s="38"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="68"/>
       <c r="C17" s="13" t="s">
         <v>172</v>
       </c>
@@ -3414,8 +3414,8 @@
       <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
-      <c r="B18" s="39" t="s">
+      <c r="A18" s="66"/>
+      <c r="B18" s="69" t="s">
         <v>199</v>
       </c>
       <c r="C18" s="16" t="s">
@@ -3431,8 +3431,8 @@
       <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
-      <c r="B19" s="37"/>
+      <c r="A19" s="66"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="10" t="s">
         <v>171</v>
       </c>
@@ -3442,8 +3442,8 @@
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="13" t="s">
         <v>172</v>
       </c>
@@ -3455,8 +3455,8 @@
       <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
-      <c r="B21" s="39" t="s">
+      <c r="A21" s="66"/>
+      <c r="B21" s="69" t="s">
         <v>200</v>
       </c>
       <c r="C21" s="16" t="s">
@@ -3470,8 +3470,8 @@
       <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
-      <c r="B22" s="37"/>
+      <c r="A22" s="66"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="10" t="s">
         <v>171</v>
       </c>
@@ -3481,8 +3481,8 @@
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
-      <c r="B23" s="38"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="68"/>
       <c r="C23" s="13" t="s">
         <v>172</v>
       </c>
@@ -3494,8 +3494,8 @@
       <c r="G23" s="15"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
-      <c r="B24" s="37" t="s">
+      <c r="A24" s="66"/>
+      <c r="B24" s="67" t="s">
         <v>201</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -3507,8 +3507,8 @@
       <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
-      <c r="B25" s="37"/>
+      <c r="A25" s="66"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="10" t="s">
         <v>171</v>
       </c>
@@ -3520,8 +3520,8 @@
       <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="40"/>
+      <c r="A26" s="65"/>
+      <c r="B26" s="63"/>
       <c r="C26" s="19" t="s">
         <v>172</v>
       </c>
@@ -3531,10 +3531,10 @@
       <c r="G26" s="21"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="62" t="s">
         <v>198</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -3548,8 +3548,8 @@
       <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="34"/>
-      <c r="B28" s="37"/>
+      <c r="A28" s="66"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="10" t="s">
         <v>171</v>
       </c>
@@ -3559,8 +3559,8 @@
       <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="34"/>
-      <c r="B29" s="38"/>
+      <c r="A29" s="66"/>
+      <c r="B29" s="68"/>
       <c r="C29" s="13" t="s">
         <v>172</v>
       </c>
@@ -3574,8 +3574,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="34"/>
-      <c r="B30" s="39" t="s">
+      <c r="A30" s="66"/>
+      <c r="B30" s="69" t="s">
         <v>199</v>
       </c>
       <c r="C30" s="16" t="s">
@@ -3593,8 +3593,8 @@
       <c r="G30" s="18"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="34"/>
-      <c r="B31" s="37"/>
+      <c r="A31" s="66"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="10" t="s">
         <v>171</v>
       </c>
@@ -3604,8 +3604,8 @@
       <c r="G31" s="12"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="34"/>
-      <c r="B32" s="38"/>
+      <c r="A32" s="66"/>
+      <c r="B32" s="68"/>
       <c r="C32" s="13" t="s">
         <v>172</v>
       </c>
@@ -3619,8 +3619,8 @@
       <c r="G32" s="15"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="34"/>
-      <c r="B33" s="39" t="s">
+      <c r="A33" s="66"/>
+      <c r="B33" s="69" t="s">
         <v>200</v>
       </c>
       <c r="C33" s="16" t="s">
@@ -3636,8 +3636,8 @@
       <c r="G33" s="18"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="34"/>
-      <c r="B34" s="37"/>
+      <c r="A34" s="66"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="10" t="s">
         <v>171</v>
       </c>
@@ -3647,8 +3647,8 @@
       <c r="G34" s="12"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="34"/>
-      <c r="B35" s="38"/>
+      <c r="A35" s="66"/>
+      <c r="B35" s="68"/>
       <c r="C35" s="13" t="s">
         <v>172</v>
       </c>
@@ -3662,8 +3662,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="34"/>
-      <c r="B36" s="37" t="s">
+      <c r="A36" s="66"/>
+      <c r="B36" s="67" t="s">
         <v>201</v>
       </c>
       <c r="C36" s="10" t="s">
@@ -3677,8 +3677,8 @@
       <c r="G36" s="12"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="34"/>
-      <c r="B37" s="37"/>
+      <c r="A37" s="66"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="10" t="s">
         <v>171</v>
       </c>
@@ -3688,8 +3688,8 @@
       <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="65"/>
+      <c r="B38" s="63"/>
       <c r="C38" s="19" t="s">
         <v>172</v>
       </c>
@@ -3702,11 +3702,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A14"/>
     <mergeCell ref="A27:A38"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B8"/>
@@ -3721,6 +3716,11 @@
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="B27:B29"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A14"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:G38">
     <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="High">
@@ -3748,185 +3748,185 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="43" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="43" customWidth="1"/>
-    <col min="3" max="3" width="21" style="43" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" style="43" customWidth="1"/>
-    <col min="5" max="6" width="25.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="43" customWidth="1"/>
-    <col min="9" max="9" width="43.28515625" style="43" customWidth="1"/>
-    <col min="10" max="10" width="33.7109375" style="43" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="43"/>
+    <col min="1" max="1" width="17.140625" style="32" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="21" style="32" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="32" customWidth="1"/>
+    <col min="5" max="6" width="25.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" style="32" customWidth="1"/>
+    <col min="9" max="9" width="43.28515625" style="32" customWidth="1"/>
+    <col min="10" max="10" width="33.7109375" style="32" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="72" t="s">
         <v>213</v>
       </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="69"/>
-    </row>
-    <row r="2" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="62" t="s">
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="74"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="78"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="54" t="s">
         <v>166</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="E2" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="54" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="54" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="80" t="s">
+      <c r="E3" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="78" t="s">
+      <c r="F3" s="54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81"/>
-      <c r="B4" s="74" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="70"/>
+      <c r="B4" s="52" t="s">
         <v>171</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="74" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="74" t="s">
+      <c r="F4" s="52" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="82"/>
-      <c r="B5" s="75" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="71"/>
+      <c r="B5" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
         <v>169</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="54" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="C6" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="78" t="s">
+      <c r="D6" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="80" t="s">
+      <c r="E6" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="83"/>
-    </row>
-    <row r="7" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="81"/>
-      <c r="B7" s="74" t="s">
+      <c r="F6" s="56"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="70"/>
+      <c r="B7" s="52" t="s">
         <v>171</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="62" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="84"/>
-    </row>
-    <row r="8" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="82"/>
-      <c r="B8" s="75" t="s">
+      <c r="F7" s="57"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="71"/>
+      <c r="B8" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="47" t="s">
+      <c r="C8" s="34"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="85"/>
-    </row>
-    <row r="9" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="81" t="s">
+      <c r="F8" s="58"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="70" t="s">
         <v>170</v>
       </c>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="52" t="s">
         <v>173</v>
       </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="74" t="s">
+      <c r="C9" s="43"/>
+      <c r="D9" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="84"/>
-    </row>
-    <row r="10" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="81"/>
-      <c r="B10" s="74" t="s">
+      <c r="F9" s="57"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="70"/>
+      <c r="B10" s="52" t="s">
         <v>171</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="62" t="s">
+      <c r="C10" s="43"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="84"/>
-    </row>
-    <row r="11" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="82"/>
-      <c r="B11" s="75" t="s">
+      <c r="F10" s="57"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="71"/>
+      <c r="B11" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="75" t="s">
+      <c r="C11" s="34"/>
+      <c r="D11" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="85"/>
+      <c r="F11" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3951,358 +3951,358 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="43.140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.7109375" style="45" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="45"/>
+    <col min="1" max="1" width="10.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="43.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.7109375" style="33" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="80" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="75" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="72" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="69"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="74"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="55" t="s">
+      <c r="A2" s="81"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="39" t="s">
         <v>216</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="35" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+    <row r="3" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="51" t="s">
+      <c r="C3" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="37" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="50" t="s">
+    <row r="4" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="84"/>
+      <c r="B4" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" s="71" t="s">
+      <c r="C4" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="E4" s="51"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="50" t="s">
+      <c r="A5" s="84"/>
+      <c r="B5" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="51" t="s">
+      <c r="C5" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="49"/>
+      <c r="E5" s="37" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="50" t="s">
+      <c r="A6" s="84"/>
+      <c r="B6" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="51"/>
+      <c r="C6" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="49"/>
+      <c r="E6" s="37"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="50" t="s">
+      <c r="A7" s="84"/>
+      <c r="B7" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="C7" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D7" s="71" t="s">
+      <c r="C7" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="E7" s="51"/>
+      <c r="E7" s="37"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
-      <c r="B8" s="50" t="s">
+      <c r="A8" s="84"/>
+      <c r="B8" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="C8" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" s="71"/>
-      <c r="E8" s="51"/>
+      <c r="C8" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="49"/>
+      <c r="E8" s="37"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="50" t="s">
+      <c r="A9" s="84"/>
+      <c r="B9" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="C9" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D9" s="71" t="s">
+      <c r="C9" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="E9" s="51"/>
+      <c r="E9" s="37"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="54"/>
-      <c r="B10" s="55" t="s">
+      <c r="A10" s="85"/>
+      <c r="B10" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="C10" s="65" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" s="72" t="s">
+      <c r="C10" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="E10" s="56"/>
+      <c r="E10" s="40"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="75" t="s">
         <v>182</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="C11" s="66" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" s="73"/>
-      <c r="E11" s="59" t="s">
+      <c r="C11" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="51"/>
+      <c r="E11" s="42" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="60"/>
-      <c r="B12" s="50" t="s">
+      <c r="A12" s="76"/>
+      <c r="B12" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="C12" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D12" s="71" t="s">
+      <c r="C12" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="37"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="60"/>
-      <c r="B13" s="50" t="s">
+      <c r="A13" s="76"/>
+      <c r="B13" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C13" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D13" s="71"/>
-      <c r="E13" s="51" t="s">
+      <c r="C13" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="49"/>
+      <c r="E13" s="37" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="60"/>
-      <c r="B14" s="50" t="s">
+      <c r="A14" s="76"/>
+      <c r="B14" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="C14" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D14" s="71"/>
-      <c r="E14" s="51"/>
+      <c r="C14" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" s="49"/>
+      <c r="E14" s="37"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="60"/>
-      <c r="B15" s="50" t="s">
+      <c r="A15" s="76"/>
+      <c r="B15" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="C15" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D15" s="71" t="s">
+      <c r="C15" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="E15" s="51"/>
+      <c r="E15" s="37"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
-      <c r="B16" s="50" t="s">
+      <c r="A16" s="76"/>
+      <c r="B16" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="C16" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="71"/>
-      <c r="E16" s="51"/>
+      <c r="C16" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="49"/>
+      <c r="E16" s="37"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="60"/>
-      <c r="B17" s="50" t="s">
+      <c r="A17" s="76"/>
+      <c r="B17" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="C17" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" s="71" t="s">
+      <c r="C17" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="E17" s="51"/>
+      <c r="E17" s="37"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
-      <c r="B18" s="55" t="s">
+      <c r="A18" s="82"/>
+      <c r="B18" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="C18" s="65" t="s">
-        <v>129</v>
-      </c>
-      <c r="D18" s="72" t="s">
+      <c r="C18" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="E18" s="56"/>
+      <c r="E18" s="40"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="75" t="s">
         <v>183</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="C19" s="66" t="s">
-        <v>129</v>
-      </c>
-      <c r="D19" s="73"/>
-      <c r="E19" s="59" t="s">
+      <c r="C19" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="51"/>
+      <c r="E19" s="42" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="60"/>
-      <c r="B20" s="50" t="s">
+      <c r="A20" s="76"/>
+      <c r="B20" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="C20" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D20" s="71" t="s">
+      <c r="C20" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="E20" s="51"/>
+      <c r="E20" s="37"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="60"/>
-      <c r="B21" s="50" t="s">
+      <c r="A21" s="76"/>
+      <c r="B21" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C21" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D21" s="71" t="s">
+      <c r="C21" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="E21" s="51" t="s">
+      <c r="E21" s="37" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="60"/>
-      <c r="B22" s="50" t="s">
+      <c r="A22" s="76"/>
+      <c r="B22" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="C22" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="D22" s="74"/>
-      <c r="E22" s="63"/>
+      <c r="C22" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" s="52"/>
+      <c r="E22" s="44"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="60"/>
-      <c r="B23" s="50" t="s">
+      <c r="A23" s="76"/>
+      <c r="B23" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="C23" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="D23" s="74" t="s">
+      <c r="C23" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="E23" s="63"/>
+      <c r="E23" s="44"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="60"/>
-      <c r="B24" s="50" t="s">
+      <c r="A24" s="76"/>
+      <c r="B24" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="C24" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" s="74"/>
-      <c r="E24" s="63"/>
+      <c r="C24" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="52"/>
+      <c r="E24" s="44"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="60"/>
-      <c r="B25" s="50" t="s">
+      <c r="A25" s="76"/>
+      <c r="B25" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="C25" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" s="74" t="s">
+      <c r="C25" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="E25" s="63" t="s">
+      <c r="E25" s="44" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="61"/>
-      <c r="B26" s="55" t="s">
+      <c r="A26" s="82"/>
+      <c r="B26" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="C26" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" s="75" t="s">
+      <c r="C26" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="E26" s="48"/>
+      <c r="E26" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A19:A26"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A19:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>